<commit_message>
Fix test for not depending on TimeSpan serialization precision
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataValidationTime.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataValidationTime.xlsx
@@ -378,45 +378,45 @@
   <x:sheetData>
     <x:row r="1" spans="1:2">
       <x:c r="A1" s="1" t="n">
-        <x:v>0.0416666666666667</x:v>
+        <x:v>0.25</x:v>
       </x:c>
       <x:c r="B1" s="1" t="n">
-        <x:v>0.104166666666667</x:v>
+        <x:v>0.5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:dataValidations count="16">
     <x:dataValidation type="time" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A2:A10">
-      <x:formula1>0.041666666666666664</x:formula1>
+      <x:formula1>0.25</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="time" errorStyle="stop" operator="notEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B10">
-      <x:formula1>0.041666666666666664</x:formula1>
+      <x:formula1>0.25</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="time" errorStyle="stop" operator="greaterThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C2:C10">
-      <x:formula1>0.041666666666666664</x:formula1>
+      <x:formula1>0.25</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="time" errorStyle="stop" operator="lessThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D2:D10">
-      <x:formula1>0.041666666666666664</x:formula1>
+      <x:formula1>0.25</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="time" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E2:E10">
-      <x:formula1>0.041666666666666664</x:formula1>
+      <x:formula1>0.25</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="time" errorStyle="stop" operator="lessThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F2:F10">
-      <x:formula1>0.041666666666666664</x:formula1>
+      <x:formula1>0.25</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="time" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G2:G10">
-      <x:formula1>0.041666666666666664</x:formula1>
-      <x:formula2>0.10416666666666667</x:formula2>
+      <x:formula1>0.25</x:formula1>
+      <x:formula2>0.5</x:formula2>
     </x:dataValidation>
     <x:dataValidation type="time" errorStyle="stop" operator="notBetween" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="H2:H10">
-      <x:formula1>0.041666666666666664</x:formula1>
-      <x:formula2>0.10416666666666667</x:formula2>
+      <x:formula1>0.25</x:formula1>
+      <x:formula2>0.5</x:formula2>
     </x:dataValidation>
     <x:dataValidation type="time" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A20">
       <x:formula1>$A$1</x:formula1>

</xml_diff>